<commit_message>
Code refatoring for modularity
</commit_message>
<xml_diff>
--- a/google_alerts_news.xlsx
+++ b/google_alerts_news.xlsx
@@ -753,901 +753,901 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; slips as markets weigh impact of US-Iran talks, &lt;b&gt;demand&lt;/b&gt; | Reuters</t>
+          <t>Natural Gas, WTI &lt;b&gt;Oil&lt;/b&gt;, Brent &lt;b&gt;Oil&lt;/b&gt; Forecasts – Geopolitics Lift &lt;b&gt;Crude&lt;/b&gt;; Gas Slumps on Mild Weather</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-prices-rise-signs-faltering-us-iran-nuclear-talks-2025-05-20/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0C-UnL2dV-ias2N4NwSnRt</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/natural-gas-wti-oil-brent-oil-forecasts-geopolitics-lift-crude-gas-slumps-on-mild-weather-1520138&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3MzKWvJTEnxY5POCP03blP</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1747720948</v>
+        <v>1747751114</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; settles up as signs of US-Iran impasse counter economic concerns | Reuters</t>
+          <t>US shale to plateau if &lt;b&gt;oil&lt;/b&gt; stays in current range, ConocoPhillips CEO says | Reuters</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-little-changed-investors-eye-iran-us-talks-china-data-2025-05-19/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0Qu-VDlPofuN2D1Z67-bxQ</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/business/energy/us-shale-plateau-if-oil-prices-stay-current-range-conocophillips-ceo-says-2025-05-20/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1dtQWTod0lgrDUdD1R3UhH</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1747719439</v>
+        <v>1747748643</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>7 Energy Winners in a Market Going Nowhere | OilPrice.com</t>
+          <t>IEA revised historical &lt;b&gt;oil&lt;/b&gt; demand data, can we trust the numbers? Is this &lt;b&gt;price&lt;/b&gt; manipulation?</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Energy-General/7-Energy-Winners-in-a-Market-Going-Nowhere.html&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3iUxJM5HIM6KaCayrvkBsC</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://energynewsbeat.co/iea-revised-historical-oil-demand-data-can-we-trust-the-numbers-is-this-price-manipulation/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3QV1jIPC9JDq2JIKiP4xGZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1747719162</v>
+        <v>1747747757</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; Ends Higher After Volatile Day Amid Ukraine Ceasefire Talks - Yahoo Finance</t>
+          <t>Exclusive-Kazakhstan's &lt;b&gt;oil&lt;/b&gt; output rises 2% in May in defiance of OPEC+ - Yahoo Finance</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/oil-falls-trump-says-ukraine-180009443.html&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0EpYqWPcLjh4Rr2huJfMsx</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/exclusive-kazakhstans-oil-output-rises-134659859.html&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2GKX459yrv2YojLhnMpVP2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1747719109</v>
+        <v>1747745564</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; Prices Drop as U.S. Loses Top AAA Rating | OilPrice.com</t>
+          <t>Natural Gas and &lt;b&gt;Oil&lt;/b&gt; Forecast: Moody's Downgrade and China Data Cloud &lt;b&gt;Price&lt;/b&gt; Outlook</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Oil-Prices/Oil-Prices-Drop-as-US-Loses-Top-AAA-Rating.html&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0p6X_xQS2ZCfiFXfNQgC-t</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/natural-gas-and-oil-forecast-moodys-downgrade-and-china-data-cloud-price-outlook-1520211&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2_olf4Hn2F5gGZ-hxwBCO4</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1747719083</v>
+        <v>1747745285</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Natural Gas, WTI &lt;b&gt;Oil&lt;/b&gt;, Brent &lt;b&gt;Oil&lt;/b&gt; Forecasts – Geopolitics Lift &lt;b&gt;Crude&lt;/b&gt;; Gas Slumps on Mild Weather</t>
+          <t>Russia's war of aggression against Ukraine: EU agrees 17th package of sanctions</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/natural-gas-wti-oil-brent-oil-forecasts-geopolitics-lift-crude-gas-slumps-on-mild-weather-1520138&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3MzKWvJTEnxY5POCP03blP</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.consilium.europa.eu/en/press/press-releases/2025/05/20/russia-s-war-of-aggression-against-ukraine-eu-agrees-17th-package-of-sanctions/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2EmlZiS94TuQrPm6E5CNs8</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1747718366</v>
+        <v>1747741269</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; Edges Down as Trump Retreats From Ukraine-Russia Peace Talks - Bloomberg</t>
+          <t>Kuwait &lt;b&gt;oil price&lt;/b&gt; up 49 cents to $64.66 pb - ZAWYA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.bloomberg.com/news/articles/2025-05-19/latest-oil-market-news-and-analysis-for-may-20&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw06T_UcjFWGOXou4wxiAN2o</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.zawya.com/en/economy/gcc/kuwait-oil-price-up-49-cents-to-6466-pb-pswe9yj3&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2_d8Qy5ByLPrv67HVQs6Fq</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1747717986</v>
+        <v>1747740885</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Southeastern Gabar &lt;b&gt;oil&lt;/b&gt; field now covers 8% of Türkiye's &lt;b&gt;demand&lt;/b&gt; | Daily Sabah</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; Markets at a Crossroads: Brent and WTI Struggle Near Key Technical Level</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.dailysabah.com/business/energy/southeastern-gabar-oil-field-now-covers-8-of-turkiyes-demand&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1_tM4DTqksWi-48Zh7F6GQ</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.riotimesonline.com/oil-markets-at-a-crossroads-brent-and-wti-struggle-near-key-technical-level/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw26AP5lB5JstJXodnqtOqrY</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1747717707</v>
+        <v>1747740785</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; edges higher on signs of US-Iran nuclear deal breakdown - Seeking Alpha</t>
+          <t>U.S. shale output nearing peak as &lt;b&gt;oil prices&lt;/b&gt; stagnate - Oil &amp;amp; Gas 360</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://seekingalpha.com/news/4450295-oil-edges-higher-on-signs-of-us-iran-nuclear-deal-breakdown&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw20GXziTim3hvDJRU7yHBmC</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.oilandgas360.com/u-s-shale-output-nearing-peak-as-oil-prices-stagnate/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2egRjnY1BgNESKUmbfTT11</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1747716999</v>
+        <v>1747740205</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Top 5 African countries that produced the most &lt;b&gt;oil&lt;/b&gt; in April 2025 | Business Insider Africa</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; Edges Lower Amid Geopolitical Uncertainty, Demand Concerns - WSJ</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://africa.businessinsider.com/local/markets/top-5-african-countries-that-produced-the-most-oil-in-april-2025/9p6js66&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw39niFLkDx9vAFwOmr1Ic4l</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.wsj.com/finance/commodities-futures/oil-edges-higher-amid-easing-supply-worries-1322ed02&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0O00yWEtgOKnLVgMnrDKtd</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1747715459</v>
+        <v>1747739664</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Crude Oil&lt;/b&gt; Recovers After Chinese Data, Goldman Upgrade - MarketPulse</t>
+          <t>Bakken Oil Threatened by &lt;b&gt;Oil Price&lt;/b&gt; Decline | 342125 - Industrial Info Resources</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.marketpulse.com/markets/crude-oil-recovers-after-chinese-data-goldman-upgrade/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2h_DGyxdZYqfLsuF6e3qjp</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.industrialinfo.com/news/abstract/bakken-oil-threatened-by-oil-price-decline--342125&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0h4k_I1DJ7Amer9mhXZgu0</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1747711359</v>
+        <v>1747735838</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Expected data center &lt;b&gt;demand&lt;/b&gt; drives up gas company valuations</t>
+          <t>OPEC Report: &lt;b&gt;Crude Oil Prices&lt;/b&gt; Decline Amid Hedge Fund Sell-Off, Demand Growth Forecasted</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mrt.com/business/oil/article/natural-gas-data-center-demand-20335611.php&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw07YUlC6ulqrlR7kitNDPdM</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://channel8.com/english/news/33794&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw31gFigfuqxq6Oiwj2N5whh</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1747709548</v>
+        <v>1747733869</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Dealing with propane &lt;b&gt;demand&lt;/b&gt; volatility - LP Gas Magazine</t>
+          <t>Avocados, &lt;b&gt;oil&lt;/b&gt;, 401(k)s: How global markets hit your wallet - Yahoo Finance</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.lpgasmagazine.com/dealing-with-propane-demand-volatility/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2fNrztYJrAG4OnOoa5LpAb</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/video/avocados-oil-401-k-global-100051372.html&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0I9EAZbtZPoxaPF4_eNjDA</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1747709310</v>
+        <v>1747731830</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Rupee Rises Against US Dollar Amid Weak Greenback and &lt;b&gt;Oil&lt;/b&gt; Prices - India News Network</t>
+          <t>7 Energy Winners in a Market Going Nowhere | OilPrice.com</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.indianewsnetwork.com/en/20250519/rupee-rises-against-us-dollar-amid-weak-greenback-and-oil-prices&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1OXn7fnWOoVZL78-eg3KVZ</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Energy-General/7-Energy-Winners-in-a-Market-Going-Nowhere.html&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3iUxJM5HIM6KaCayrvkBsC</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1747707548</v>
+        <v>1747730198</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Don't Stop Believin' - Is the Marcellus/Utica Finally Poised for a Gas-Production Breakout?</t>
+          <t>&lt;b&gt;Crude Oil price&lt;/b&gt; today: WTI price bearish at European opening - Mitrade</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://rbnenergy.com/dont-stop-believin-is-the-marcellus-utica-finally-poised-for-a-gas-production-breakout&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1NzNaMpzBiCC2nWKUv_Py_</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mitrade.com/insights/news/live-news/article-2-830437-20250520&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2rkH3RFxXWyapBwOTsW5oE</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1747707312</v>
+        <v>1747729773</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Crystal Flash claims state workplace award - Bulk Transporter</t>
+          <t>Forecasting equity risk premium: the role of investor concern on &lt;b&gt;oil price&lt;/b&gt; volatility</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.bulktransporter.com/fleet-management/article/55291155/crystal-flash-claims-workplace-award-in-michigan&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw18zpZLSnOM6RVMXhR7o05Y</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.sciencedirect.com/science/article/abs/pii/S0275531925002466&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw15iXUkno8zANe87mGAfwG7</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1747700208</v>
+        <v>1747729444</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Georgia Gas Price Average speeds Upward at the Pumps - WNEG</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; slips as markets weigh impact of US-Iran talks, demand | Reuters</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://wnegradio.com/georgia-gas-price-average-speeds-upward-at-the-pumps/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2Q-04skytf11IuevVxI-Nz</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-prices-rise-signs-faltering-us-iran-nuclear-talks-2025-05-20/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0C-UnL2dV-ias2N4NwSnRt</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1747697747</v>
+        <v>1747726348</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>IEA: Global &lt;b&gt;oil demand&lt;/b&gt; growth is slowing - SAFETY4SEA</t>
+          <t>INTERVIEW: African &lt;b&gt;oil&lt;/b&gt; trader Mocoh seeks second life as Dangote squeezes flows</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://safety4sea.com/iea-global-oil-demand-growth-is-slowing/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw104qbdnIdJGwvwaLdQfdKL</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.spglobal.com/commodity-insights/en/news-research/latest-news/refined-products/051925-interview-african-oil-trader-mocoh-seeks-second-life-as-dangote-squeezes-flows&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1QP4OKlwONCjYRdttXoNSz</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1747697176</v>
+        <v>1747724024</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Georgia gas prices rise as &lt;b&gt;crude oil&lt;/b&gt; costs and &lt;b&gt;demand&lt;/b&gt; climb - Cobb Courier</t>
+          <t>&lt;b&gt;Crude Oil price&lt;/b&gt; today: WTI price bearish at European opening - Mitrade</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://cobbcountycourier.com/2025/05/georgia-gas-prices-rise-as-crude-oil-costs-and-demand-climb/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2raTtNOAxU4WDuSfb59Edr</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mitrade.com/au/insights/news/live-news/article-2-830437-20250520&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1aGVb2vriy1j7EatuUrfMw</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1747696939</v>
+        <v>1747721377</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Balances: Supply Surplus Widens Ahead of Peak Summer &lt;b&gt;Demand&lt;/b&gt; | Energy Intelligence</t>
+          <t>The rise of the credit card airport lounge : The Indicator from Planet Money - NPR</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.energyintel.com/00000196-5a0c-d3bc-a5ff-dbfcd67a0001&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1rh3xovitpYRPrjepS8jNf</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.npr.org/2025/05/20/1252436007/the-rise-of-the-credit-card-airport-lounge&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3Msq6z92kjWiNgjwOWUCX0</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1747686664</v>
+        <v>1747721002</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bakken Oil Threatened by &lt;b&gt;Oil Price&lt;/b&gt; Decline | 342125 - Industrial Info Resources</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; slips as markets weigh impact of US-Iran talks, &lt;b&gt;demand&lt;/b&gt; | Reuters</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.industrialinfo.com/news/abstract/bakken-oil-threatened-by-oil-price-decline--342125&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0h4k_I1DJ7Amer9mhXZgu0</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-prices-rise-signs-faltering-us-iran-nuclear-talks-2025-05-20/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0C-UnL2dV-ias2N4NwSnRt</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1747735838</v>
+        <v>1747720948</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>EU reportedly to lower &lt;b&gt;price&lt;/b&gt; cap on Russian &lt;b&gt;oil&lt;/b&gt; at G7 meeting in Canada</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; settles up as signs of US-Iran impasse counter economic concerns | Reuters</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://euromaidanpress.com/2025/05/20/eu-reportedly-to-lower-price-cap-on-russian-oil-at-g7-meeting-in-canada/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2uswOBirnbmRhbmJJLPVee</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-little-changed-investors-eye-iran-us-talks-china-data-2025-05-19/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0Qu-VDlPofuN2D1Z67-bxQ</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1747734781</v>
+        <v>1747719439</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Natural Gas and &lt;b&gt;Oil&lt;/b&gt; Forecast: Moody's Downgrade and China Data Cloud &lt;b&gt;Price&lt;/b&gt; Outlook</t>
+          <t>7 Energy Winners in a Market Going Nowhere | OilPrice.com</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/natural-gas-and-oil-forecast-moodys-downgrade-and-china-data-cloud-price-outlook-1520211&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2_olf4Hn2F5gGZ-hxwBCO4</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Energy-General/7-Energy-Winners-in-a-Market-Going-Nowhere.html&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3iUxJM5HIM6KaCayrvkBsC</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1747734396</v>
+        <v>1747719162</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Crude &lt;b&gt;Oil Prices&lt;/b&gt; Supported by Dollar Weakness and Iran Nuclear Deal Doubts - Nasdaq</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; Ends Higher After Volatile Day Amid Ukraine Ceasefire Talks - Yahoo Finance</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.nasdaq.com/articles/crude-oil-prices-supported-dollar-weakness-and-iran-nuclear-deal-doubts&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2updotlPM4wmRBP2rL5SZe</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/oil-falls-trump-says-ukraine-180009443.html&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0EpYqWPcLjh4Rr2huJfMsx</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1747734210</v>
+        <v>1747719109</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>OPEC Report: Crude &lt;b&gt;Oil Prices&lt;/b&gt; Decline Amid Hedge Fund Sell-Off, Demand Growth Forecasted</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; Prices Drop as U.S. Loses Top AAA Rating | OilPrice.com</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://channel8.com/english/news/33794&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw31gFigfuqxq6Oiwj2N5whh</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Oil-Prices/Oil-Prices-Drop-as-US-Loses-Top-AAA-Rating.html&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0p6X_xQS2ZCfiFXfNQgC-t</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1747733869</v>
+        <v>1747719083</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Kuwait &lt;b&gt;oil price&lt;/b&gt; up 49 cents to $64.66 pb - ZAWYA</t>
+          <t>Natural Gas, WTI &lt;b&gt;Oil&lt;/b&gt;, Brent &lt;b&gt;Oil&lt;/b&gt; Forecasts – Geopolitics Lift &lt;b&gt;Crude&lt;/b&gt;; Gas Slumps on Mild Weather</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.zawya.com/en/economy/gcc/kuwait-oil-price-up-49-cents-to-6466-pb-pswe9yj3&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2_d8Qy5ByLPrv67HVQs6Fq</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/natural-gas-wti-oil-brent-oil-forecasts-geopolitics-lift-crude-gas-slumps-on-mild-weather-1520138&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3MzKWvJTEnxY5POCP03blP</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1747733526</v>
+        <v>1747718366</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Avocados, &lt;b&gt;oil&lt;/b&gt;, 401(k)s: How global markets hit your wallet - Yahoo Finance</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; Edges Down as Trump Retreats From Ukraine-Russia Peace Talks - Bloomberg</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/video/avocados-oil-401-k-global-100051372.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0I9EAZbtZPoxaPF4_eNjDA</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.bloomberg.com/news/articles/2025-05-19/latest-oil-market-news-and-analysis-for-may-20&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw06T_UcjFWGOXou4wxiAN2o</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1747731830</v>
+        <v>1747717986</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Forecasting equity risk premium: the role of investor concern on &lt;b&gt;oil price&lt;/b&gt; volatility</t>
+          <t>Southeastern Gabar &lt;b&gt;oil&lt;/b&gt; field now covers 8% of Türkiye's &lt;b&gt;demand&lt;/b&gt; | Daily Sabah</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.sciencedirect.com/science/article/abs/pii/S0275531925002466&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw15iXUkno8zANe87mGAfwG7</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.dailysabah.com/business/energy/southeastern-gabar-oil-field-now-covers-8-of-turkiyes-demand&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1_tM4DTqksWi-48Zh7F6GQ</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1747729444</v>
+        <v>1747717707</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>SASOL FACTS</t>
+          <t>&lt;b&gt;Oil&lt;/b&gt; edges higher on signs of US-Iran nuclear deal breakdown - Seeking Alpha</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.sasol.com/sites/default/files/2025-05/Sasol%2520Fact%2520Sheet%2520%257C%2520Understanding%2520the%2520breakeven%2520oil%2520price%2520for%2520Southern%2520Africa.pdf&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw30QxNlI1JgaBXm2x1iWAfz</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://seekingalpha.com/news/4450295-oil-edges-higher-on-signs-of-us-iran-nuclear-deal-breakdown&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw20GXziTim3hvDJRU7yHBmC</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1747728743</v>
+        <v>1747716999</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>US shale to plateau if &lt;b&gt;oil prices&lt;/b&gt; stay in current range, ConocoPhillips CEO says - Yahoo Finance</t>
+          <t>Top 5 African countries that produced the most &lt;b&gt;oil&lt;/b&gt; in April 2025 | Business Insider Africa</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/us-shale-plateau-oil-prices-084110532.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0i4IOhFpWNi9tNHZ4Is_uy</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://africa.businessinsider.com/local/markets/top-5-african-countries-that-produced-the-most-oil-in-april-2025/9p6js66&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw39niFLkDx9vAFwOmr1Ic4l</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1747728014</v>
+        <v>1747715459</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>OPEC's Moves Hit &lt;b&gt;Oil Prices&lt;/b&gt; While Demand Stays Strong - Finimize</t>
+          <t>&lt;b&gt;Crude Oil&lt;/b&gt; Recovers After Chinese Data, Goldman Upgrade - MarketPulse</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finimize.com/content/opecs-moves-hit-oil-prices-while-demand-stays-strong&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1PjeKVtIRrjxiS9kCXzyaO</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.marketpulse.com/markets/crude-oil-recovers-after-chinese-data-goldman-upgrade/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2h_DGyxdZYqfLsuF6e3qjp</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1747724728</v>
+        <v>1747711359</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Undervalued FCF kings : r/ValueInvesting - Reddit</t>
+          <t>Expected data center &lt;b&gt;demand&lt;/b&gt; drives up gas company valuations</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reddit.com/r/ValueInvesting/comments/1kqg0pg/undervalued_fcf_kings/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3AWydo9yH13K7Gzavobv4B</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mrt.com/business/oil/article/natural-gas-data-center-demand-20335611.php&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw07YUlC6ulqrlR7kitNDPdM</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1747724245</v>
+        <v>1747709548</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Cheap Indonesia Suppliers Solid Vegetable Refined Palm Cooking &lt;b&gt;Oil Price&lt;/b&gt; - Alibaba</t>
+          <t>Dealing with propane &lt;b&gt;demand&lt;/b&gt; volatility - LP Gas Magazine</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.alibaba.com/product-detail/Cheap-Indonesia-Suppliers-Solid-Vegetable-Refined_60713298312.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1EqwjMTeopZPG3CI5bcm02</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.lpgasmagazine.com/dealing-with-propane-demand-volatility/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2fNrztYJrAG4OnOoa5LpAb</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1747723449</v>
+        <v>1747709310</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>The oil market is still gutted and &lt;b&gt;crude price&lt;/b&gt; is nowhere near the triple dollar mark that ... - Facebook</t>
+          <t>Rupee Rises Against US Dollar Amid Weak Greenback and &lt;b&gt;Oil&lt;/b&gt; Prices - India News Network</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://m.facebook.com/thehindu/posts/the-oil-market-is-still-gutted-and-crude-price-is-nowhere-near-the-triple-dollar/1010033981327986/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1dqRiX7loRCMQ26FX56p6E</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.indianewsnetwork.com/en/20250519/rupee-rises-against-us-dollar-amid-weak-greenback-and-oil-prices&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1OXn7fnWOoVZL78-eg3KVZ</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1747722923</v>
+        <v>1747707548</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DAVID KOENIG | The Seattle Times | Page 99</t>
+          <t>Don't Stop Believin' - Is the Marcellus/Utica Finally Poised for a Gas-Production Breakout?</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.seattletimes.com/author/david-koenig/page/99/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0THYxnWc2W675KBP5cEtWL</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://rbnenergy.com/dont-stop-believin-is-the-marcellus-utica-finally-poised-for-a-gas-production-breakout&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1NzNaMpzBiCC2nWKUv_Py_</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1747721893</v>
+        <v>1747707312</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt;, Natural Gas, and US Dollar Technical Analysis: Global Risk and Geopolitics Limit Upside</t>
+          <t>Crystal Flash claims state workplace award - Bulk Transporter</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/oil-natural-gas-and-us-dollar-technical-analysis-global-risk-and-geopolitics-limit-upside-1520176&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3lDNcoThnS-M6gF55ck0pc</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.bulktransporter.com/fleet-management/article/55291155/crystal-flash-claims-workplace-award-in-michigan&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw18zpZLSnOM6RVMXhR7o05Y</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1747721747</v>
+        <v>1747700208</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>The rise of the credit card airport lounge : The Indicator from Planet Money - NPR</t>
+          <t>Georgia Gas Price Average speeds Upward at the Pumps - WNEG</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.npr.org/2025/05/20/1252436007/the-rise-of-the-credit-card-airport-lounge&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3Msq6z92kjWiNgjwOWUCX0</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://wnegradio.com/georgia-gas-price-average-speeds-upward-at-the-pumps/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2Q-04skytf11IuevVxI-Nz</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1747721002</v>
+        <v>1747697747</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; slips as markets weigh impact of US-Iran talks, demand | Reuters</t>
+          <t>IEA: Global &lt;b&gt;oil demand&lt;/b&gt; growth is slowing - SAFETY4SEA</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-prices-rise-signs-faltering-us-iran-nuclear-talks-2025-05-20/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0C-UnL2dV-ias2N4NwSnRt</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://safety4sea.com/iea-global-oil-demand-growth-is-slowing/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw104qbdnIdJGwvwaLdQfdKL</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1747720948</v>
+        <v>1747697176</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Citi Downgrades Patterson-UTI, Helmerich &amp;amp; Payne On &lt;b&gt;Oil Price&lt;/b&gt; Risk - MSN</t>
+          <t>Georgia gas prices rise as &lt;b&gt;crude oil&lt;/b&gt; costs and &lt;b&gt;demand&lt;/b&gt; climb - Cobb Courier</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.msn.com/en-us/money/markets/citi-downgrades-patterson-uti-helmerich-payne-on-oil-price-risk-retail-surprised-by-brutal-selloff/ar-AA1F6FQ2%3Focid%3Dfinance-verthp-feeds&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3HuUgukk9UopmvREIybEr_</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://cobbcountycourier.com/2025/05/georgia-gas-prices-rise-as-crude-oil-costs-and-demand-climb/&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2raTtNOAxU4WDuSfb59Edr</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1747720770</v>
+        <v>1747696939</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7 Energy Winners in a Market Going Nowhere | &lt;b&gt;OilPrice&lt;/b&gt;.com</t>
+          <t>Balances: Supply Surplus Widens Ahead of Peak Summer &lt;b&gt;Demand&lt;/b&gt; | Energy Intelligence</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Energy-General/7-Energy-Winners-in-a-Market-Going-Nowhere.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3iUxJM5HIM6KaCayrvkBsC</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.energyintel.com/00000196-5a0c-d3bc-a5ff-dbfcd67a0001&amp;ct=ga&amp;cd=CAIyHGRlYTExMGJiZDM3Njg2YmI6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1rh3xovitpYRPrjepS8jNf</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1747719162</v>
+        <v>1747686664</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>U.S. shale output nearing peak as &lt;b&gt;oil prices&lt;/b&gt; stagnate - Oil &amp;amp; Gas 360</t>
+          <t>Expert Reveals Trumps Plan for the Middle East &amp;amp; Why &lt;b&gt;Oil Price&lt;/b&gt; Is About to Explode</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.oilandgas360.com/u-s-shale-output-nearing-peak-as-oil-prices-stagnate/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2egRjnY1BgNESKUmbfTT11</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.realclearenergy.org/video/2025/05/20/expert_reveals_trumps_plan_for_the_middle_east_and_why_oil_price_is_about_to_explode_1111432.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw23e2q58foaEWY21tAo8_AG</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1747740205</v>
+        <v>1747748971</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7 Energy Winners in a Market Going Nowhere | OilPrice.com</t>
+          <t>Russia's war of aggression against Ukraine: EU agrees 17th package of sanctions</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Energy-General/7-Energy-Winners-in-a-Market-Going-Nowhere.html&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3iUxJM5HIM6KaCayrvkBsC</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.consilium.europa.eu/en/press/press-releases/2025/05/20/russia-s-war-of-aggression-against-ukraine-eu-agrees-17th-package-of-sanctions/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2EmlZiS94TuQrPm6E5CNs8</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1747730198</v>
+        <v>1747748437</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Crude Oil price&lt;/b&gt; today: WTI price bearish at European opening - Mitrade</t>
+          <t>&lt;b&gt;Oil Prices&lt;/b&gt; Remain Rangebound as Geopolitical Catalysts Loom | &lt;b&gt;OilPrice&lt;/b&gt;.com</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mitrade.com/insights/news/live-news/article-2-830437-20250520&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2rkH3RFxXWyapBwOTsW5oE</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://oilprice.com/Energy/Energy-General/Oil-Prices-Remain-Rangebound-as-Geopolitical-Catalysts-Loom.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3NaDUmMbb2-wmMG3JZJ-tP</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1747729773</v>
+        <v>1747746221</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil&lt;/b&gt; slips as markets weigh impact of US-Iran talks, demand | Reuters</t>
+          <t>EU Plans New Sanctions on Russia in Push for Ukraine Cease-fire - The New York Times</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reuters.com/markets/commodities/oil-prices-rise-signs-faltering-us-iran-nuclear-talks-2025-05-20/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0C-UnL2dV-ias2N4NwSnRt</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.nytimes.com/2025/05/20/world/europe/european-union-russia-sanctions.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1qVSpQnQdWbukgHVrEaxPf</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1747726348</v>
+        <v>1747745349</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>INTERVIEW: African &lt;b&gt;oil&lt;/b&gt; trader Mocoh seeks second life as Dangote squeezes flows</t>
+          <t>Javier Blas - X</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.spglobal.com/commodity-insights/en/news-research/latest-news/refined-products/051925-interview-african-oil-trader-mocoh-seeks-second-life-as-dangote-squeezes-flows&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1QP4OKlwONCjYRdttXoNSz</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://x.com/JavierBlas/status/1924781012900340076&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3Z8wzQnbYZ-gKGV_q8qciW</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1747724024</v>
+        <v>1747740046</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Crude Oil price&lt;/b&gt; today: WTI price bearish at European opening - Mitrade</t>
+          <t>Naeem Aslam on X: &amp;quot;G7 MULLS LOWER RUSSIA &lt;b&gt;OIL PRICE&lt;/b&gt; CAP The UK confirms G7 talks ...</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mitrade.com/au/insights/news/live-news/article-2-830437-20250520&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1aGVb2vriy1j7EatuUrfMw</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://twitter.com/NaeemAslam23/status/1924781372616417618&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1jUJQdqXFfqTzbTve8HTYU</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1747721377</v>
+        <v>1747737470</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>The rise of the credit card airport lounge : The Indicator from Planet Money - NPR</t>
+          <t>The &lt;b&gt;oil price&lt;/b&gt; conundrum: Tackling market risk with analyst Tamas Varga | TP ICAP</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.npr.org/2025/05/20/1252436007/the-rise-of-the-credit-card-airport-lounge&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3Msq6z92kjWiNgjwOWUCX0</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.linkedin.com/posts/tp-icap_the-oil-price-conundrum-tackling-market-activity-7330529448359792640-yBzG&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2oTnHbVQo84JsaacLDsR81</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1747721002</v>
+        <v>1747737095</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Citi Downgrades Patterson-UTI, Helmerich &amp;amp; Payne On &lt;b&gt;Oil Price&lt;/b&gt; Risk - MSN</t>
+          <t>Bakken Oil Threatened by &lt;b&gt;Oil Price&lt;/b&gt; Decline | 342125 - Industrial Info Resources</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.msn.com/en-us/money/markets/citi-downgrades-patterson-uti-helmerich-payne-on-oil-price-risk-retail-surprised-by-brutal-selloff/ar-AA1F6FQ2%3Focid%3Dfinance-verthp-feeds&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3HuUgukk9UopmvREIybEr_</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.industrialinfo.com/news/abstract/bakken-oil-threatened-by-oil-price-decline--342125&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0h4k_I1DJ7Amer9mhXZgu0</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1747720770</v>
+        <v>1747735838</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Despite the fluctuations in global &lt;b&gt;crude oil prices&lt;/b&gt;, Dangote Petroleum Refinery ...</t>
+          <t>EU reportedly to lower &lt;b&gt;price&lt;/b&gt; cap on Russian &lt;b&gt;oil&lt;/b&gt; at G7 meeting in Canada</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://m.facebook.com/vanguardngr/posts/despite-the-fluctuations-in-global-crude-oil-prices-dangote-petroleum-refinery-p/1151127793726338/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1NIfyBD3ljSIgQYOEHo9G2</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://euromaidanpress.com/2025/05/20/eu-reportedly-to-lower-price-cap-on-russian-oil-at-g7-meeting-in-canada/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2uswOBirnbmRhbmJJLPVee</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1747719186</v>
+        <v>1747734781</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Citi Downgrades Patterson-UTI, Helmerich &amp;amp; Payne On &lt;b&gt;Oil Price&lt;/b&gt; Risk - Stocktwits</t>
+          <t>Natural Gas and &lt;b&gt;Oil&lt;/b&gt; Forecast: Moody's Downgrade and China Data Cloud &lt;b&gt;Price&lt;/b&gt; Outlook</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://stocktwits.com/news-articles/markets/equity/citi-downgrades-patterson-uti-helmerich-and-payne-on-oil-price-risk/ch0dF7jRb8M&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1hTrZ6SiP6KbYooNtBSKH5</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.fxempire.com/forecasts/article/natural-gas-and-oil-forecast-moodys-downgrade-and-china-data-cloud-price-outlook-1520211&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2_olf4Hn2F5gGZ-hxwBCO4</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1747718994</v>
+        <v>1747734396</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Oil prices&lt;/b&gt; fall on China/U.S. economic worries; Ukraine peace talks eyed - Oil &amp;amp; Gas 360</t>
+          <t>Crude &lt;b&gt;Oil Prices&lt;/b&gt; Supported by Dollar Weakness and Iran Nuclear Deal Doubts - Nasdaq</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.oilandgas360.com/oil-prices-fall-on-china-u-s-economic-worries-ukraine-peace-talks-eyed/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1MZw-olsTZJCXLMs099C0i</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.nasdaq.com/articles/crude-oil-prices-supported-dollar-weakness-and-iran-nuclear-deal-doubts&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2updotlPM4wmRBP2rL5SZe</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1747717995</v>
+        <v>1747734210</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Future of North Dakota drilling facing uncertainty amid &lt;b&gt;pricing&lt;/b&gt; fluctuation - McKenzie County Farmer</t>
+          <t>OPEC Report: Crude &lt;b&gt;Oil Prices&lt;/b&gt; Decline Amid Hedge Fund Sell-Off, Demand Growth Forecasted</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=http://www.watfordcitynd.com/latest-news/future-of-north-dakota-drilling-facing-uncertainty-amid-pricing-fluctuation/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2kgFBnu3t_A9R1ARbIJRR8</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://channel8.com/english/news/33794&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw31gFigfuqxq6Oiwj2N5whh</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1747716430</v>
+        <v>1747733869</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>INDONESIA &lt;b&gt;CRUDE PRICE&lt;/b&gt; EXPECTED AT $60-$80/BARREL IN 2026&amp;quot; / X</t>
+          <t>Kuwait &lt;b&gt;oil price&lt;/b&gt; up 49 cents to $64.66 pb - ZAWYA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://x.com/PiQSuite/status/1924677518742946042&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1bkZw6Uq9fFDVHtw92Goki</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.zawya.com/en/economy/gcc/kuwait-oil-price-up-49-cents-to-6466-pb-pswe9yj3&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2_d8Qy5ByLPrv67HVQs6Fq</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1747710295</v>
+        <v>1747733526</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Crude Oil Prices&lt;/b&gt; Hold Firm On Uncertainty On US-Iran Trade Negotiations - YouTube</t>
+          <t>Avocados, &lt;b&gt;oil&lt;/b&gt;, 401(k)s: How global markets hit your wallet - Yahoo Finance</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.youtube.com/watch%3Fv%3Dn3VM8gf6jPc&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3irrP95lxIi4euFbmJ7XtQ</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/video/avocados-oil-401-k-global-100051372.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0I9EAZbtZPoxaPF4_eNjDA</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1747705861</v>
+        <v>1747731830</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>GCC Sovereigns' &lt;b&gt;Oil Price&lt;/b&gt; Vulnerabilities - Events</t>
+          <t>Forecasting equity risk premium: the role of investor concern on &lt;b&gt;oil price&lt;/b&gt; volatility</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://events.fitchratings.com/gccsovereignsoilpricevulnerabi&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw20v2qaniOhj3pVCrTlJVRc</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.sciencedirect.com/science/article/abs/pii/S0275531925002466&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw15iXUkno8zANe87mGAfwG7</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1747705274</v>
+        <v>1747729444</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Propane Expensive Relative to &lt;b&gt;Crude Oil&lt;/b&gt; – Likely to Continue for 2025 | RBN Energy</t>
+          <t>SASOL FACTS</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://rbnenergy.com/analyst-insights/propane-expensive-relative-crude-oil-%25E2%2580%2593-likely-continue-2025&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1r0LPp67xrYw8-eTzn0rIu</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.sasol.com/sites/default/files/2025-05/Sasol%2520Fact%2520Sheet%2520%257C%2520Understanding%2520the%2520breakeven%2520oil%2520price%2520for%2520Southern%2520Africa.pdf&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw30QxNlI1JgaBXm2x1iWAfz</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1747705023</v>
+        <v>1747728743</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>EU to push G7 to lower Russian &lt;b&gt;oil price&lt;/b&gt; cap, commissioner says - The Kyiv Independent</t>
+          <t>US shale to plateau if &lt;b&gt;oil prices&lt;/b&gt; stay in current range, ConocoPhillips CEO says - Yahoo Finance</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://kyivindependent.com/eu-to-push-g7-to-lower-russian-oil-price-cap-commissioner-says/&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw01bHMejYwqGhmhXdI9Pzn8</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finance.yahoo.com/news/us-shale-plateau-oil-prices-084110532.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw0i4IOhFpWNi9tNHZ4Is_uy</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1747704508</v>
+        <v>1747728014</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Crude Oil price&lt;/b&gt; today: WTI price bearish at European opening - Mitrade</t>
+          <t>OPEC's Moves Hit &lt;b&gt;Oil Prices&lt;/b&gt; While Demand Stays Strong - Finimize</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.mitrade.com/au/insights/news/live-news/article-2-828352-20250519&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw2-jM5ehGTV69dkjpIiBJpS</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://finimize.com/content/opecs-moves-hit-oil-prices-while-demand-stays-strong&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1PjeKVtIRrjxiS9kCXzyaO</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1747703264</v>
+        <v>1747724728</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>&lt;b&gt;Crude Oil&lt;/b&gt; Futures Contract Specs - CME Group</t>
+          <t>Undervalued FCF kings : r/ValueInvesting - Reddit</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.cmegroup.com/markets/energy/crude-oil/light-sweet-crude.contractSpecs.html%3Fredirect%3D/trading/energy/light-sweet-crude-oil/wti-houston-crude-oil-futures.html%26videoId%3D6372861444112&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3VN_ZmH5gw56-cf-Lq0FTH</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.reddit.com/r/ValueInvesting/comments/1kqg0pg/undervalued_fcf_kings/&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw3AWydo9yH13K7Gzavobv4B</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1747698855</v>
+        <v>1747724245</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CommSec on X: &amp;quot;The Brent &lt;b&gt;crude price&lt;/b&gt; gained US13 cents or 0.2% to US$65.54 a barrel ...</t>
+          <t>Cheap Indonesia Suppliers Solid Vegetable Refined Palm Cooking &lt;b&gt;Oil Price&lt;/b&gt; - Alibaba</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://x.com/CommSec/status/1924575266892136884&amp;ct=ga&amp;cd=CAIyHGI1YTY5MjliYjhiNDYxNzY6Y29tOmVuOlVTOlI&amp;usg=AOvVaw089Rw4wtUpy-tsdX087b5k</t>
+          <t>https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.alibaba.com/product-detail/Cheap-Indonesia-Suppliers-Solid-Vegetable-Refined_60713298312.html&amp;ct=ga&amp;cd=CAIyHDE4Mzk5ODdlN2JhNTdiMTA6Y29tOmVuOlVTOlI&amp;usg=AOvVaw1EqwjMTeopZPG3CI5bcm02</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1747691290</v>
+        <v>1747723449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>